<commit_message>
experiment1 vFinal + newdata
</commit_message>
<xml_diff>
--- a/Jasper Files/data/addNP/addNP-100pod-50pol.xlsx
+++ b/Jasper Files/data/addNP/addNP-100pod-50pol.xlsx
@@ -516,28 +516,28 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.02873167023062706</v>
+        <v>0.05179256305564195</v>
       </c>
       <c r="C2">
-        <v>489927</v>
+        <v>617717</v>
       </c>
       <c r="D2">
-        <v>650771</v>
+        <v>781516</v>
       </c>
       <c r="E2">
-        <v>160844</v>
+        <v>163799</v>
       </c>
       <c r="F2">
-        <v>0.006362222135066986</v>
+        <v>0.02593199908733368</v>
       </c>
       <c r="G2">
-        <v>35537</v>
+        <v>39439</v>
       </c>
       <c r="H2">
-        <v>78009</v>
+        <v>81163</v>
       </c>
       <c r="I2">
-        <v>42472</v>
+        <v>41724</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -545,28 +545,28 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.02955982089042664</v>
+        <v>0.05827882001176476</v>
       </c>
       <c r="C3">
-        <v>443471</v>
+        <v>1004093</v>
       </c>
       <c r="D3">
-        <v>608717</v>
+        <v>1079031</v>
       </c>
       <c r="E3">
-        <v>165246</v>
+        <v>74938</v>
       </c>
       <c r="F3">
-        <v>0.007177781313657761</v>
+        <v>0.01665396697353572</v>
       </c>
       <c r="G3">
-        <v>35274</v>
+        <v>36672</v>
       </c>
       <c r="H3">
-        <v>77615</v>
+        <v>79144</v>
       </c>
       <c r="I3">
-        <v>42341</v>
+        <v>42472</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -574,28 +574,28 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.02177886292338371</v>
+        <v>0.05567719705868512</v>
       </c>
       <c r="C4">
-        <v>348305</v>
+        <v>707792</v>
       </c>
       <c r="D4">
-        <v>597352</v>
+        <v>784335</v>
       </c>
       <c r="E4">
-        <v>249047</v>
+        <v>76543</v>
       </c>
       <c r="F4">
-        <v>0.006096221506595612</v>
+        <v>0.02302647894248366</v>
       </c>
       <c r="G4">
-        <v>34433</v>
+        <v>35679</v>
       </c>
       <c r="H4">
-        <v>76929</v>
+        <v>78021</v>
       </c>
       <c r="I4">
-        <v>42496</v>
+        <v>42342</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -603,28 +603,28 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.02629760652780533</v>
+        <v>0.03252339095342904</v>
       </c>
       <c r="C5">
-        <v>344850</v>
+        <v>714012</v>
       </c>
       <c r="D5">
-        <v>523058</v>
+        <v>875708</v>
       </c>
       <c r="E5">
-        <v>178208</v>
+        <v>161696</v>
       </c>
       <c r="F5">
-        <v>0.006620410829782486</v>
+        <v>0.00856433401349932</v>
       </c>
       <c r="G5">
-        <v>34931</v>
+        <v>36465</v>
       </c>
       <c r="H5">
-        <v>77274</v>
+        <v>78961</v>
       </c>
       <c r="I5">
-        <v>42343</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -632,28 +632,28 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.03306474536657333</v>
+        <v>0.03343780804425478</v>
       </c>
       <c r="C6">
-        <v>485237</v>
+        <v>662030</v>
       </c>
       <c r="D6">
-        <v>641085</v>
+        <v>821982</v>
       </c>
       <c r="E6">
-        <v>155848</v>
+        <v>159952</v>
       </c>
       <c r="F6">
-        <v>0.006494820117950439</v>
+        <v>0.0166499960469082</v>
       </c>
       <c r="G6">
-        <v>34849</v>
+        <v>36105</v>
       </c>
       <c r="H6">
-        <v>77321</v>
+        <v>78601</v>
       </c>
       <c r="I6">
-        <v>42472</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -661,25 +661,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.02228819951415062</v>
+        <v>0.05424914590548724</v>
       </c>
       <c r="C7">
-        <v>361431</v>
+        <v>930747</v>
       </c>
       <c r="D7">
-        <v>525604</v>
+        <v>1094563</v>
       </c>
       <c r="E7">
-        <v>164173</v>
+        <v>163816</v>
       </c>
       <c r="F7">
-        <v>0.009749062359333038</v>
+        <v>0.02747824206016958</v>
       </c>
       <c r="G7">
-        <v>35169</v>
+        <v>36445</v>
       </c>
       <c r="H7">
-        <v>77665</v>
+        <v>78941</v>
       </c>
       <c r="I7">
         <v>42496</v>
@@ -690,25 +690,25 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.04181357845664024</v>
+        <v>0.02880557300522923</v>
       </c>
       <c r="C8">
-        <v>461137</v>
+        <v>224634</v>
       </c>
       <c r="D8">
-        <v>624308</v>
+        <v>384818</v>
       </c>
       <c r="E8">
-        <v>163171</v>
+        <v>160184</v>
       </c>
       <c r="F8">
-        <v>0.01050077378749847</v>
+        <v>0.02301052096299827</v>
       </c>
       <c r="G8">
-        <v>34689</v>
+        <v>36735</v>
       </c>
       <c r="H8">
-        <v>77185</v>
+        <v>79231</v>
       </c>
       <c r="I8">
         <v>42496</v>
@@ -719,28 +719,28 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.02401032298803329</v>
+        <v>0.02343337808270007</v>
       </c>
       <c r="C9">
-        <v>364121</v>
+        <v>231823</v>
       </c>
       <c r="D9">
-        <v>628074</v>
+        <v>395769</v>
       </c>
       <c r="E9">
-        <v>263953</v>
+        <v>163946</v>
       </c>
       <c r="F9">
-        <v>0.006895687431097031</v>
+        <v>0.02924754098057747</v>
       </c>
       <c r="G9">
-        <v>35713</v>
+        <v>36255</v>
       </c>
       <c r="H9">
-        <v>78209</v>
+        <v>78593</v>
       </c>
       <c r="I9">
-        <v>42496</v>
+        <v>42338</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -748,25 +748,25 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.02800415828824043</v>
+        <v>0.0468835219508037</v>
       </c>
       <c r="C10">
-        <v>476969</v>
+        <v>498486</v>
       </c>
       <c r="D10">
-        <v>635915</v>
+        <v>722412</v>
       </c>
       <c r="E10">
-        <v>158946</v>
+        <v>223926</v>
       </c>
       <c r="F10">
-        <v>0.009527258574962616</v>
+        <v>0.03188073798082769</v>
       </c>
       <c r="G10">
-        <v>35297</v>
+        <v>36959</v>
       </c>
       <c r="H10">
-        <v>77793</v>
+        <v>79455</v>
       </c>
       <c r="I10">
         <v>42496</v>
@@ -777,28 +777,28 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.05884800106287003</v>
+        <v>0.029354277998209</v>
       </c>
       <c r="C11">
-        <v>358097</v>
+        <v>291319</v>
       </c>
       <c r="D11">
-        <v>579604</v>
+        <v>528258</v>
       </c>
       <c r="E11">
-        <v>221507</v>
+        <v>236939</v>
       </c>
       <c r="F11">
-        <v>0.006241988390684128</v>
+        <v>0.00868447998072952</v>
       </c>
       <c r="G11">
-        <v>34804</v>
+        <v>36690</v>
       </c>
       <c r="H11">
-        <v>77145</v>
+        <v>79033</v>
       </c>
       <c r="I11">
-        <v>42341</v>
+        <v>42343</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -806,28 +806,28 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.02705815434455872</v>
+        <v>0.04446813801769167</v>
       </c>
       <c r="C12">
-        <v>345394</v>
+        <v>663514</v>
       </c>
       <c r="D12">
-        <v>506674</v>
+        <v>824652</v>
       </c>
       <c r="E12">
-        <v>161280</v>
+        <v>161138</v>
       </c>
       <c r="F12">
-        <v>0.00766034796833992</v>
+        <v>0.01543714106082916</v>
       </c>
       <c r="G12">
-        <v>34209</v>
+        <v>36415</v>
       </c>
       <c r="H12">
-        <v>76551</v>
+        <v>78911</v>
       </c>
       <c r="I12">
-        <v>42342</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -835,28 +835,28 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.0273890495300293</v>
+        <v>0.0225869850255549</v>
       </c>
       <c r="C13">
-        <v>360428</v>
+        <v>236819</v>
       </c>
       <c r="D13">
-        <v>614810</v>
+        <v>400367</v>
       </c>
       <c r="E13">
-        <v>254382</v>
+        <v>163548</v>
       </c>
       <c r="F13">
-        <v>0.006271190941333771</v>
+        <v>0.03360715392045677</v>
       </c>
       <c r="G13">
-        <v>34945</v>
+        <v>37055</v>
       </c>
       <c r="H13">
-        <v>77441</v>
+        <v>79397</v>
       </c>
       <c r="I13">
-        <v>42496</v>
+        <v>42342</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -864,28 +864,28 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.02412807568907738</v>
+        <v>0.04290584498085082</v>
       </c>
       <c r="C14">
-        <v>360179</v>
+        <v>689265</v>
       </c>
       <c r="D14">
-        <v>634348</v>
+        <v>849665</v>
       </c>
       <c r="E14">
-        <v>274169</v>
+        <v>160400</v>
       </c>
       <c r="F14">
-        <v>0.006741456687450409</v>
+        <v>0.02746228105388582</v>
       </c>
       <c r="G14">
-        <v>34913</v>
+        <v>36951</v>
       </c>
       <c r="H14">
-        <v>77409</v>
+        <v>79423</v>
       </c>
       <c r="I14">
-        <v>42496</v>
+        <v>42472</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -893,28 +893,28 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.01135098561644554</v>
+        <v>0.04121529404073954</v>
       </c>
       <c r="C15">
-        <v>218513</v>
+        <v>682774</v>
       </c>
       <c r="D15">
-        <v>373681</v>
+        <v>847460</v>
       </c>
       <c r="E15">
-        <v>155168</v>
+        <v>164686</v>
       </c>
       <c r="F15">
-        <v>0.008117921650409698</v>
+        <v>0.01787809398956597</v>
       </c>
       <c r="G15">
-        <v>35137</v>
+        <v>36383</v>
       </c>
       <c r="H15">
-        <v>77475</v>
+        <v>78414</v>
       </c>
       <c r="I15">
-        <v>42338</v>
+        <v>42031</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -922,28 +922,28 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.01502466574311256</v>
+        <v>0.02109930606093258</v>
       </c>
       <c r="C16">
-        <v>231600</v>
+        <v>268952</v>
       </c>
       <c r="D16">
-        <v>426954</v>
+        <v>428343</v>
       </c>
       <c r="E16">
-        <v>195354</v>
+        <v>159391</v>
       </c>
       <c r="F16">
-        <v>0.006459206342697144</v>
+        <v>0.02564465103205293</v>
       </c>
       <c r="G16">
-        <v>35233</v>
+        <v>36639</v>
       </c>
       <c r="H16">
-        <v>77729</v>
+        <v>78825</v>
       </c>
       <c r="I16">
-        <v>42496</v>
+        <v>42186</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -951,28 +951,28 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.03014221414923668</v>
+        <v>0.03428756701759994</v>
       </c>
       <c r="C17">
-        <v>435649</v>
+        <v>779785</v>
       </c>
       <c r="D17">
-        <v>594353</v>
+        <v>872742</v>
       </c>
       <c r="E17">
-        <v>158704</v>
+        <v>92957</v>
       </c>
       <c r="F17">
-        <v>0.006434988230466843</v>
+        <v>0.0262744938954711</v>
       </c>
       <c r="G17">
-        <v>34561</v>
+        <v>36351</v>
       </c>
       <c r="H17">
-        <v>77057</v>
+        <v>78689</v>
       </c>
       <c r="I17">
-        <v>42496</v>
+        <v>42338</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -980,28 +980,28 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.02794639393687248</v>
+        <v>0.05343281896784902</v>
       </c>
       <c r="C18">
-        <v>349573</v>
+        <v>806258</v>
       </c>
       <c r="D18">
-        <v>520340</v>
+        <v>969286</v>
       </c>
       <c r="E18">
-        <v>170767</v>
+        <v>163028</v>
       </c>
       <c r="F18">
-        <v>0.006607271730899811</v>
+        <v>0.02501561399549246</v>
       </c>
       <c r="G18">
-        <v>34593</v>
+        <v>36351</v>
       </c>
       <c r="H18">
-        <v>77089</v>
+        <v>78690</v>
       </c>
       <c r="I18">
-        <v>42496</v>
+        <v>42339</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1009,25 +1009,25 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.02183426544070244</v>
+        <v>0.03418757696636021</v>
       </c>
       <c r="C19">
-        <v>350010</v>
+        <v>239061</v>
       </c>
       <c r="D19">
-        <v>598985</v>
+        <v>474924</v>
       </c>
       <c r="E19">
-        <v>248975</v>
+        <v>235863</v>
       </c>
       <c r="F19">
-        <v>0.00680319219827652</v>
+        <v>0.01830620400141925</v>
       </c>
       <c r="G19">
-        <v>35457</v>
+        <v>36895</v>
       </c>
       <c r="H19">
-        <v>77953</v>
+        <v>79391</v>
       </c>
       <c r="I19">
         <v>42496</v>
@@ -1038,28 +1038,28 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.01564854010939598</v>
+        <v>0.02491042600013316</v>
       </c>
       <c r="C20">
-        <v>229464</v>
+        <v>254403</v>
       </c>
       <c r="D20">
-        <v>392312</v>
+        <v>417243</v>
       </c>
       <c r="E20">
-        <v>162848</v>
+        <v>162840</v>
       </c>
       <c r="F20">
-        <v>0.006557393819093704</v>
+        <v>0.02548066398594528</v>
       </c>
       <c r="G20">
-        <v>35385</v>
+        <v>36287</v>
       </c>
       <c r="H20">
-        <v>77857</v>
+        <v>78783</v>
       </c>
       <c r="I20">
-        <v>42472</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1067,25 +1067,25 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.01675904542207718</v>
+        <v>0.05100494693033397</v>
       </c>
       <c r="C21">
-        <v>220285</v>
+        <v>809713</v>
       </c>
       <c r="D21">
-        <v>380429</v>
+        <v>975113</v>
       </c>
       <c r="E21">
-        <v>160144</v>
+        <v>165400</v>
       </c>
       <c r="F21">
-        <v>0.006721649318933487</v>
+        <v>0.02244535298086703</v>
       </c>
       <c r="G21">
-        <v>34273</v>
+        <v>35423</v>
       </c>
       <c r="H21">
-        <v>76769</v>
+        <v>77919</v>
       </c>
       <c r="I21">
         <v>42496</v>
@@ -1096,28 +1096,28 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.0286383219063282</v>
+        <v>0.0237183190183714</v>
       </c>
       <c r="C22">
-        <v>359595</v>
+        <v>251715</v>
       </c>
       <c r="D22">
-        <v>516747</v>
+        <v>486587</v>
       </c>
       <c r="E22">
-        <v>157152</v>
+        <v>234872</v>
       </c>
       <c r="F22">
-        <v>0.006585545837879181</v>
+        <v>0.02286038000602275</v>
       </c>
       <c r="G22">
-        <v>34911</v>
+        <v>36293</v>
       </c>
       <c r="H22">
-        <v>77383</v>
+        <v>78789</v>
       </c>
       <c r="I22">
-        <v>42472</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1125,25 +1125,25 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.02866209670901299</v>
+        <v>0.02545940096024424</v>
       </c>
       <c r="C23">
-        <v>426481</v>
+        <v>278116</v>
       </c>
       <c r="D23">
-        <v>586156</v>
+        <v>442297</v>
       </c>
       <c r="E23">
-        <v>159675</v>
+        <v>164181</v>
       </c>
       <c r="F23">
-        <v>0.007155738770961761</v>
+        <v>0.02667567890603095</v>
       </c>
       <c r="G23">
-        <v>35393</v>
+        <v>36575</v>
       </c>
       <c r="H23">
-        <v>77889</v>
+        <v>79071</v>
       </c>
       <c r="I23">
         <v>42496</v>
@@ -1154,25 +1154,25 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.02624764293432236</v>
+        <v>0.04235905699897557</v>
       </c>
       <c r="C24">
-        <v>349916</v>
+        <v>706655</v>
       </c>
       <c r="D24">
-        <v>518471</v>
+        <v>869881</v>
       </c>
       <c r="E24">
-        <v>168555</v>
+        <v>163226</v>
       </c>
       <c r="F24">
-        <v>0.01075334101915359</v>
+        <v>0.02103989198803902</v>
       </c>
       <c r="G24">
-        <v>34753</v>
+        <v>36383</v>
       </c>
       <c r="H24">
-        <v>77249</v>
+        <v>78879</v>
       </c>
       <c r="I24">
         <v>42496</v>
@@ -1183,25 +1183,25 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.0110054723918438</v>
+        <v>0.05552478705067188</v>
       </c>
       <c r="C25">
-        <v>224101</v>
+        <v>443153</v>
       </c>
       <c r="D25">
-        <v>384493</v>
+        <v>605086</v>
       </c>
       <c r="E25">
-        <v>160392</v>
+        <v>161933</v>
       </c>
       <c r="F25">
-        <v>0.006060302257537842</v>
+        <v>0.03421278507448733</v>
       </c>
       <c r="G25">
-        <v>35033</v>
+        <v>37111</v>
       </c>
       <c r="H25">
-        <v>77505</v>
+        <v>79583</v>
       </c>
       <c r="I25">
         <v>42472</v>
@@ -1212,28 +1212,28 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.048305943608284</v>
+        <v>0.05382156802807003</v>
       </c>
       <c r="C26">
-        <v>467189</v>
+        <v>821128</v>
       </c>
       <c r="D26">
-        <v>624385</v>
+        <v>984234</v>
       </c>
       <c r="E26">
-        <v>157196</v>
+        <v>163106</v>
       </c>
       <c r="F26">
-        <v>0.011625986546278</v>
+        <v>0.02318558096885681</v>
       </c>
       <c r="G26">
-        <v>35233</v>
+        <v>36511</v>
       </c>
       <c r="H26">
-        <v>77729</v>
+        <v>78852</v>
       </c>
       <c r="I26">
-        <v>42496</v>
+        <v>42341</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1241,28 +1241,28 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.03133812174201012</v>
+        <v>0.05698129802476615</v>
       </c>
       <c r="C27">
-        <v>362213</v>
+        <v>968036</v>
       </c>
       <c r="D27">
-        <v>521874</v>
+        <v>1129328</v>
       </c>
       <c r="E27">
-        <v>159661</v>
+        <v>161292</v>
       </c>
       <c r="F27">
-        <v>0.006481561809778214</v>
+        <v>0.02588394202757627</v>
       </c>
       <c r="G27">
-        <v>34625</v>
+        <v>36863</v>
       </c>
       <c r="H27">
-        <v>77121</v>
+        <v>79203</v>
       </c>
       <c r="I27">
-        <v>42496</v>
+        <v>42340</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1270,28 +1270,28 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.01708653941750526</v>
+        <v>0.03433359402697533</v>
       </c>
       <c r="C28">
-        <v>352981</v>
+        <v>794144</v>
       </c>
       <c r="D28">
-        <v>511061</v>
+        <v>957510</v>
       </c>
       <c r="E28">
-        <v>158080</v>
+        <v>163366</v>
       </c>
       <c r="F28">
-        <v>0.008070468902587891</v>
+        <v>0.01693498296663165</v>
       </c>
       <c r="G28">
-        <v>34081</v>
+        <v>36607</v>
       </c>
       <c r="H28">
-        <v>76419</v>
+        <v>79103</v>
       </c>
       <c r="I28">
-        <v>42338</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1299,25 +1299,25 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.03991847112774849</v>
+        <v>0.02142986794933677</v>
       </c>
       <c r="C29">
-        <v>464196</v>
+        <v>224691</v>
       </c>
       <c r="D29">
-        <v>632972</v>
+        <v>385795</v>
       </c>
       <c r="E29">
-        <v>168776</v>
+        <v>161104</v>
       </c>
       <c r="F29">
-        <v>0.008653249591588974</v>
+        <v>0.01963416498620063</v>
       </c>
       <c r="G29">
-        <v>34401</v>
+        <v>36703</v>
       </c>
       <c r="H29">
-        <v>76897</v>
+        <v>79199</v>
       </c>
       <c r="I29">
         <v>42496</v>
@@ -1328,28 +1328,28 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.03768216073513031</v>
+        <v>0.06318538496270776</v>
       </c>
       <c r="C30">
-        <v>364307</v>
+        <v>909103</v>
       </c>
       <c r="D30">
-        <v>625904</v>
+        <v>1072407</v>
       </c>
       <c r="E30">
-        <v>261597</v>
+        <v>163304</v>
       </c>
       <c r="F30">
-        <v>0.006407696753740311</v>
+        <v>0.02160429302603006</v>
       </c>
       <c r="G30">
-        <v>34433</v>
+        <v>36159</v>
       </c>
       <c r="H30">
-        <v>76774</v>
+        <v>78655</v>
       </c>
       <c r="I30">
-        <v>42341</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1357,28 +1357,28 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.02152719348669052</v>
+        <v>0.177509453962557</v>
       </c>
       <c r="C31">
-        <v>317878</v>
+        <v>711999</v>
       </c>
       <c r="D31">
-        <v>479088</v>
+        <v>876145</v>
       </c>
       <c r="E31">
-        <v>161210</v>
+        <v>164146</v>
       </c>
       <c r="F31">
-        <v>0.009604018181562424</v>
+        <v>0.01513753202743828</v>
       </c>
       <c r="G31">
-        <v>35169</v>
+        <v>36991</v>
       </c>
       <c r="H31">
-        <v>77665</v>
+        <v>79329</v>
       </c>
       <c r="I31">
-        <v>42496</v>
+        <v>42338</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1386,28 +1386,28 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.03217069059610367</v>
+        <v>0.0533926059724763</v>
       </c>
       <c r="C32">
-        <v>345397</v>
+        <v>625253</v>
       </c>
       <c r="D32">
-        <v>504029</v>
+        <v>788663</v>
       </c>
       <c r="E32">
-        <v>158632</v>
+        <v>163410</v>
       </c>
       <c r="F32">
-        <v>0.006596747785806656</v>
+        <v>0.02834367100149393</v>
       </c>
       <c r="G32">
-        <v>34593</v>
+        <v>35999</v>
       </c>
       <c r="H32">
-        <v>76779</v>
+        <v>78495</v>
       </c>
       <c r="I32">
-        <v>42186</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1415,25 +1415,25 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.03657320886850357</v>
+        <v>0.05442398705054075</v>
       </c>
       <c r="C33">
-        <v>483454</v>
+        <v>507819</v>
       </c>
       <c r="D33">
-        <v>641578</v>
+        <v>664958</v>
       </c>
       <c r="E33">
-        <v>158124</v>
+        <v>157139</v>
       </c>
       <c r="F33">
-        <v>0.006259962916374207</v>
+        <v>0.02607872500084341</v>
       </c>
       <c r="G33">
-        <v>34593</v>
+        <v>36831</v>
       </c>
       <c r="H33">
-        <v>77089</v>
+        <v>79327</v>
       </c>
       <c r="I33">
         <v>42496</v>
@@ -1444,28 +1444,28 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.02364076673984528</v>
+        <v>0.06816836597863585</v>
       </c>
       <c r="C34">
-        <v>360667</v>
+        <v>826192</v>
       </c>
       <c r="D34">
-        <v>524147</v>
+        <v>989123</v>
       </c>
       <c r="E34">
-        <v>163480</v>
+        <v>162931</v>
       </c>
       <c r="F34">
-        <v>0.009160399436950684</v>
+        <v>0.01531826006248593</v>
       </c>
       <c r="G34">
-        <v>34945</v>
+        <v>36671</v>
       </c>
       <c r="H34">
-        <v>77283</v>
+        <v>79167</v>
       </c>
       <c r="I34">
-        <v>42338</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1473,28 +1473,28 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.02224266529083252</v>
+        <v>0.03345066297333688</v>
       </c>
       <c r="C35">
-        <v>238784</v>
+        <v>248778</v>
       </c>
       <c r="D35">
-        <v>404084</v>
+        <v>487119</v>
       </c>
       <c r="E35">
-        <v>165300</v>
+        <v>238341</v>
       </c>
       <c r="F35">
-        <v>0.005349114537239075</v>
+        <v>0.01768660405650735</v>
       </c>
       <c r="G35">
-        <v>34393</v>
+        <v>36567</v>
       </c>
       <c r="H35">
-        <v>76865</v>
+        <v>78882</v>
       </c>
       <c r="I35">
-        <v>42472</v>
+        <v>42315</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1502,25 +1502,25 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.01166203990578651</v>
+        <v>0.06627215200569481</v>
       </c>
       <c r="C36">
-        <v>224090</v>
+        <v>844135</v>
       </c>
       <c r="D36">
-        <v>385466</v>
+        <v>976510</v>
       </c>
       <c r="E36">
-        <v>161376</v>
+        <v>132375</v>
       </c>
       <c r="F36">
-        <v>0.006195466965436935</v>
+        <v>0.02515460399445146</v>
       </c>
       <c r="G36">
-        <v>35169</v>
+        <v>36191</v>
       </c>
       <c r="H36">
-        <v>77665</v>
+        <v>78687</v>
       </c>
       <c r="I36">
         <v>42496</v>
@@ -1531,25 +1531,25 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.02934082597494125</v>
+        <v>0.04099917900748551</v>
       </c>
       <c r="C37">
-        <v>357354</v>
+        <v>720514</v>
       </c>
       <c r="D37">
-        <v>559305</v>
+        <v>884551</v>
       </c>
       <c r="E37">
-        <v>201951</v>
+        <v>164037</v>
       </c>
       <c r="F37">
-        <v>0.005094759166240692</v>
+        <v>0.01966814801562577</v>
       </c>
       <c r="G37">
-        <v>35233</v>
+        <v>36575</v>
       </c>
       <c r="H37">
-        <v>77729</v>
+        <v>79071</v>
       </c>
       <c r="I37">
         <v>42496</v>
@@ -1560,28 +1560,28 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.02493716776371002</v>
+        <v>0.04020075802691281</v>
       </c>
       <c r="C38">
-        <v>429487</v>
+        <v>445471</v>
       </c>
       <c r="D38">
-        <v>587819</v>
+        <v>607067</v>
       </c>
       <c r="E38">
-        <v>158332</v>
+        <v>161596</v>
       </c>
       <c r="F38">
-        <v>0.006455160677433014</v>
+        <v>0.02163250895682722</v>
       </c>
       <c r="G38">
-        <v>34657</v>
+        <v>35807</v>
       </c>
       <c r="H38">
-        <v>77153</v>
+        <v>78150</v>
       </c>
       <c r="I38">
-        <v>42496</v>
+        <v>42343</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1589,25 +1589,25 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.02352581173181534</v>
+        <v>0.03994185593910515</v>
       </c>
       <c r="C39">
-        <v>353005</v>
+        <v>775078</v>
       </c>
       <c r="D39">
-        <v>512273</v>
+        <v>939011</v>
       </c>
       <c r="E39">
-        <v>159268</v>
+        <v>163933</v>
       </c>
       <c r="F39">
-        <v>0.0100637711584568</v>
+        <v>0.01162735989782959</v>
       </c>
       <c r="G39">
-        <v>34881</v>
+        <v>36575</v>
       </c>
       <c r="H39">
-        <v>77377</v>
+        <v>79071</v>
       </c>
       <c r="I39">
         <v>42496</v>
@@ -1618,28 +1618,28 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.01112485304474831</v>
+        <v>0.02802838303614408</v>
       </c>
       <c r="C40">
-        <v>220779</v>
+        <v>279451</v>
       </c>
       <c r="D40">
-        <v>380883</v>
+        <v>516708</v>
       </c>
       <c r="E40">
-        <v>160104</v>
+        <v>237257</v>
       </c>
       <c r="F40">
-        <v>0.008537795394659042</v>
+        <v>0.02564161806367338</v>
       </c>
       <c r="G40">
-        <v>35681</v>
+        <v>36735</v>
       </c>
       <c r="H40">
-        <v>78022</v>
+        <v>79073</v>
       </c>
       <c r="I40">
-        <v>42341</v>
+        <v>42338</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1647,25 +1647,25 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.0257340669631958</v>
+        <v>0.03315901197493076</v>
       </c>
       <c r="C41">
-        <v>355203</v>
+        <v>459716</v>
       </c>
       <c r="D41">
-        <v>519080</v>
+        <v>475454</v>
       </c>
       <c r="E41">
-        <v>163877</v>
+        <v>15738</v>
       </c>
       <c r="F41">
-        <v>0.008079234510660172</v>
+        <v>0.0267557529732585</v>
       </c>
       <c r="G41">
-        <v>35361</v>
+        <v>36511</v>
       </c>
       <c r="H41">
-        <v>77857</v>
+        <v>79007</v>
       </c>
       <c r="I41">
         <v>42496</v>
@@ -1676,28 +1676,28 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.03129605948925018</v>
+        <v>0.04876566107850522</v>
       </c>
       <c r="C42">
-        <v>458271</v>
+        <v>770544</v>
       </c>
       <c r="D42">
-        <v>618802</v>
+        <v>931218</v>
       </c>
       <c r="E42">
-        <v>160531</v>
+        <v>160674</v>
       </c>
       <c r="F42">
-        <v>0.008802026510238647</v>
+        <v>0.02532464300747961</v>
       </c>
       <c r="G42">
-        <v>34689</v>
+        <v>35935</v>
       </c>
       <c r="H42">
-        <v>76876</v>
+        <v>78431</v>
       </c>
       <c r="I42">
-        <v>42187</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1705,28 +1705,28 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.02812771871685982</v>
+        <v>0.04953207809012383</v>
       </c>
       <c r="C43">
-        <v>344263</v>
+        <v>783414</v>
       </c>
       <c r="D43">
-        <v>500974</v>
+        <v>946942</v>
       </c>
       <c r="E43">
-        <v>156711</v>
+        <v>163528</v>
       </c>
       <c r="F43">
-        <v>0.007465209811925888</v>
+        <v>0.02038055507000536</v>
       </c>
       <c r="G43">
-        <v>34593</v>
+        <v>36319</v>
       </c>
       <c r="H43">
-        <v>76936</v>
+        <v>78815</v>
       </c>
       <c r="I43">
-        <v>42343</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1734,25 +1734,25 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0.02925335243344307</v>
+        <v>0.0467131509212777</v>
       </c>
       <c r="C44">
-        <v>366150</v>
+        <v>781188</v>
       </c>
       <c r="D44">
-        <v>645554</v>
+        <v>941233</v>
       </c>
       <c r="E44">
-        <v>279404</v>
+        <v>160045</v>
       </c>
       <c r="F44">
-        <v>0.01532607153058052</v>
+        <v>0.02390530297998339</v>
       </c>
       <c r="G44">
-        <v>35521</v>
+        <v>36383</v>
       </c>
       <c r="H44">
-        <v>78017</v>
+        <v>78879</v>
       </c>
       <c r="I44">
         <v>42496</v>
@@ -1763,28 +1763,28 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.02997306734323502</v>
+        <v>0.04168667609337717</v>
       </c>
       <c r="C45">
-        <v>465299</v>
+        <v>288826</v>
       </c>
       <c r="D45">
-        <v>629510</v>
+        <v>527784</v>
       </c>
       <c r="E45">
-        <v>164211</v>
+        <v>238958</v>
       </c>
       <c r="F45">
-        <v>0.009133990854024887</v>
+        <v>0.02691760298330337</v>
       </c>
       <c r="G45">
-        <v>35617</v>
+        <v>36287</v>
       </c>
       <c r="H45">
-        <v>77955</v>
+        <v>78629</v>
       </c>
       <c r="I45">
-        <v>42338</v>
+        <v>42342</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1792,28 +1792,28 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0.01500650122761726</v>
+        <v>0.03659413103014231</v>
       </c>
       <c r="C46">
-        <v>231873</v>
+        <v>441163</v>
       </c>
       <c r="D46">
-        <v>391017</v>
+        <v>679216</v>
       </c>
       <c r="E46">
-        <v>159144</v>
+        <v>238053</v>
       </c>
       <c r="F46">
-        <v>0.006366346031427383</v>
+        <v>0.02492382994387299</v>
       </c>
       <c r="G46">
-        <v>34753</v>
+        <v>36631</v>
       </c>
       <c r="H46">
-        <v>77249</v>
+        <v>79103</v>
       </c>
       <c r="I46">
-        <v>42496</v>
+        <v>42472</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1821,25 +1821,25 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.02568159624934196</v>
+        <v>0.05208655598107725</v>
       </c>
       <c r="C47">
-        <v>362559</v>
+        <v>501663</v>
       </c>
       <c r="D47">
-        <v>651856</v>
+        <v>662527</v>
       </c>
       <c r="E47">
-        <v>289297</v>
+        <v>160864</v>
       </c>
       <c r="F47">
-        <v>0.009746763855218887</v>
+        <v>0.01493528601713479</v>
       </c>
       <c r="G47">
-        <v>35073</v>
+        <v>36447</v>
       </c>
       <c r="H47">
-        <v>77569</v>
+        <v>78943</v>
       </c>
       <c r="I47">
         <v>42496</v>
@@ -1850,28 +1850,28 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.02888549491763115</v>
+        <v>0.04074051801580936</v>
       </c>
       <c r="C48">
-        <v>364267</v>
+        <v>274265</v>
       </c>
       <c r="D48">
-        <v>611127</v>
+        <v>504383</v>
       </c>
       <c r="E48">
-        <v>246860</v>
+        <v>230118</v>
       </c>
       <c r="F48">
-        <v>0.007566079497337341</v>
+        <v>0.0189966670004651</v>
       </c>
       <c r="G48">
-        <v>35681</v>
+        <v>37375</v>
       </c>
       <c r="H48">
-        <v>78022</v>
+        <v>79871</v>
       </c>
       <c r="I48">
-        <v>42341</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1879,28 +1879,28 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.02533163875341415</v>
+        <v>0.03500059095676988</v>
       </c>
       <c r="C49">
-        <v>353583</v>
+        <v>778006</v>
       </c>
       <c r="D49">
-        <v>543602</v>
+        <v>940076</v>
       </c>
       <c r="E49">
-        <v>190019</v>
+        <v>162070</v>
       </c>
       <c r="F49">
-        <v>0.00694926455616951</v>
+        <v>0.02007465797942132</v>
       </c>
       <c r="G49">
-        <v>35617</v>
+        <v>37023</v>
       </c>
       <c r="H49">
-        <v>78113</v>
+        <v>79362</v>
       </c>
       <c r="I49">
-        <v>42496</v>
+        <v>42339</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1908,25 +1908,25 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.02287200465798378</v>
+        <v>0.0355062399758026</v>
       </c>
       <c r="C50">
-        <v>358498</v>
+        <v>280093</v>
       </c>
       <c r="D50">
-        <v>541220</v>
+        <v>442645</v>
       </c>
       <c r="E50">
-        <v>182722</v>
+        <v>162552</v>
       </c>
       <c r="F50">
-        <v>0.007208812981843948</v>
+        <v>0.02339654508978128</v>
       </c>
       <c r="G50">
-        <v>35361</v>
+        <v>37087</v>
       </c>
       <c r="H50">
-        <v>77857</v>
+        <v>79583</v>
       </c>
       <c r="I50">
         <v>42496</v>
@@ -1937,28 +1937,28 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.01966951787471771</v>
+        <v>0.04670161998365074</v>
       </c>
       <c r="C51">
-        <v>351743</v>
+        <v>699389</v>
       </c>
       <c r="D51">
-        <v>509055</v>
+        <v>859795</v>
       </c>
       <c r="E51">
-        <v>157312</v>
+        <v>160406</v>
       </c>
       <c r="F51">
-        <v>0.005911711603403091</v>
+        <v>0.017858367995359</v>
       </c>
       <c r="G51">
-        <v>34945</v>
+        <v>35487</v>
       </c>
       <c r="H51">
-        <v>77441</v>
+        <v>77516</v>
       </c>
       <c r="I51">
-        <v>42496</v>
+        <v>42029</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1966,28 +1966,28 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.02412392571568489</v>
+        <v>0.02840120496693999</v>
       </c>
       <c r="C52">
-        <v>349380</v>
+        <v>604231</v>
       </c>
       <c r="D52">
-        <v>506510</v>
+        <v>766086</v>
       </c>
       <c r="E52">
-        <v>157130</v>
+        <v>161855</v>
       </c>
       <c r="F52">
-        <v>0.007672388106584549</v>
+        <v>0.02150618296582252</v>
       </c>
       <c r="G52">
-        <v>35489</v>
+        <v>36223</v>
       </c>
       <c r="H52">
-        <v>77829</v>
+        <v>78719</v>
       </c>
       <c r="I52">
-        <v>42340</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1995,28 +1995,28 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.016386728733778</v>
+        <v>0.03639959497377276</v>
       </c>
       <c r="C53">
-        <v>350980</v>
+        <v>588993</v>
       </c>
       <c r="D53">
-        <v>514516</v>
+        <v>589304</v>
       </c>
       <c r="E53">
-        <v>163536</v>
+        <v>311</v>
       </c>
       <c r="F53">
-        <v>0.006840966641902924</v>
+        <v>0.02680590702220798</v>
       </c>
       <c r="G53">
-        <v>35353</v>
+        <v>36383</v>
       </c>
       <c r="H53">
-        <v>77670</v>
+        <v>78879</v>
       </c>
       <c r="I53">
-        <v>42317</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2024,28 +2024,28 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.02347085624933243</v>
+        <v>0.05386155401356518</v>
       </c>
       <c r="C54">
-        <v>351169</v>
+        <v>580094</v>
       </c>
       <c r="D54">
-        <v>506524</v>
+        <v>581050</v>
       </c>
       <c r="E54">
-        <v>155355</v>
+        <v>956</v>
       </c>
       <c r="F54">
-        <v>0.01273485645651817</v>
+        <v>0.01701119204517454</v>
       </c>
       <c r="G54">
-        <v>34657</v>
+        <v>36351</v>
       </c>
       <c r="H54">
-        <v>76999</v>
+        <v>78847</v>
       </c>
       <c r="I54">
-        <v>42342</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2053,28 +2053,28 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.03439041972160339</v>
+        <v>0.04579472704790533</v>
       </c>
       <c r="C55">
-        <v>453907</v>
+        <v>880636</v>
       </c>
       <c r="D55">
-        <v>612939</v>
+        <v>1073870</v>
       </c>
       <c r="E55">
-        <v>159032</v>
+        <v>193234</v>
       </c>
       <c r="F55">
-        <v>0.006648100912570953</v>
+        <v>0.02985725901089609</v>
       </c>
       <c r="G55">
-        <v>34305</v>
+        <v>36479</v>
       </c>
       <c r="H55">
-        <v>76801</v>
+        <v>78820</v>
       </c>
       <c r="I55">
-        <v>42496</v>
+        <v>42341</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2082,25 +2082,25 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>0.02127324044704437</v>
+        <v>0.03007083991542459</v>
       </c>
       <c r="C56">
-        <v>356747</v>
+        <v>394365</v>
       </c>
       <c r="D56">
-        <v>515349</v>
+        <v>633398</v>
       </c>
       <c r="E56">
-        <v>158602</v>
+        <v>239033</v>
       </c>
       <c r="F56">
-        <v>0.006282087415456772</v>
+        <v>0.02348806895315647</v>
       </c>
       <c r="G56">
-        <v>35329</v>
+        <v>37023</v>
       </c>
       <c r="H56">
-        <v>77825</v>
+        <v>79519</v>
       </c>
       <c r="I56">
         <v>42496</v>
@@ -2111,28 +2111,28 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0.02602861821651459</v>
+        <v>0.04561998299323022</v>
       </c>
       <c r="C57">
-        <v>486160</v>
+        <v>618060</v>
       </c>
       <c r="D57">
-        <v>647551</v>
+        <v>853485</v>
       </c>
       <c r="E57">
-        <v>161391</v>
+        <v>235425</v>
       </c>
       <c r="F57">
-        <v>0.009158894419670105</v>
+        <v>0.01743091898970306</v>
       </c>
       <c r="G57">
-        <v>35393</v>
+        <v>37247</v>
       </c>
       <c r="H57">
-        <v>77889</v>
+        <v>79586</v>
       </c>
       <c r="I57">
-        <v>42496</v>
+        <v>42339</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2140,28 +2140,28 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.02866625413298607</v>
+        <v>0.0762862809933722</v>
       </c>
       <c r="C58">
-        <v>365738</v>
+        <v>870724</v>
       </c>
       <c r="D58">
-        <v>526162</v>
+        <v>871203</v>
       </c>
       <c r="E58">
-        <v>160424</v>
+        <v>479</v>
       </c>
       <c r="F58">
-        <v>0.007580235600471497</v>
+        <v>0.02065927698276937</v>
       </c>
       <c r="G58">
-        <v>35129</v>
+        <v>36951</v>
       </c>
       <c r="H58">
-        <v>77601</v>
+        <v>79269</v>
       </c>
       <c r="I58">
-        <v>42472</v>
+        <v>42318</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2169,28 +2169,28 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0.037969671189785</v>
+        <v>0.0472514609573409</v>
       </c>
       <c r="C59">
-        <v>471288</v>
+        <v>653033</v>
       </c>
       <c r="D59">
-        <v>630465</v>
+        <v>814728</v>
       </c>
       <c r="E59">
-        <v>159177</v>
+        <v>161695</v>
       </c>
       <c r="F59">
-        <v>0.01171816512942314</v>
+        <v>0.02767488500103354</v>
       </c>
       <c r="G59">
-        <v>35041</v>
+        <v>36375</v>
       </c>
       <c r="H59">
-        <v>77383</v>
+        <v>78847</v>
       </c>
       <c r="I59">
-        <v>42342</v>
+        <v>42472</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2198,28 +2198,28 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0.01372860744595528</v>
+        <v>0.06048993906006217</v>
       </c>
       <c r="C60">
-        <v>229668</v>
+        <v>571444</v>
       </c>
       <c r="D60">
-        <v>392110</v>
+        <v>758902</v>
       </c>
       <c r="E60">
-        <v>162442</v>
+        <v>187458</v>
       </c>
       <c r="F60">
-        <v>0.008403882384300232</v>
+        <v>0.02648395800497383</v>
       </c>
       <c r="G60">
-        <v>34945</v>
+        <v>37279</v>
       </c>
       <c r="H60">
-        <v>77287</v>
+        <v>79775</v>
       </c>
       <c r="I60">
-        <v>42342</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2227,28 +2227,28 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.02374588698148727</v>
+        <v>0.06383508804719895</v>
       </c>
       <c r="C61">
-        <v>337622</v>
+        <v>632099</v>
       </c>
       <c r="D61">
-        <v>498622</v>
+        <v>793376</v>
       </c>
       <c r="E61">
-        <v>161000</v>
+        <v>161277</v>
       </c>
       <c r="F61">
-        <v>0.007028818130493164</v>
+        <v>0.0169299190165475</v>
       </c>
       <c r="G61">
-        <v>34753</v>
+        <v>36383</v>
       </c>
       <c r="H61">
-        <v>77095</v>
+        <v>78879</v>
       </c>
       <c r="I61">
-        <v>42342</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2256,28 +2256,28 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.02961228415369987</v>
+        <v>0.03681961901020259</v>
       </c>
       <c r="C62">
-        <v>495482</v>
+        <v>257960</v>
       </c>
       <c r="D62">
-        <v>656420</v>
+        <v>492880</v>
       </c>
       <c r="E62">
-        <v>160938</v>
+        <v>234920</v>
       </c>
       <c r="F62">
-        <v>0.006894908845424652</v>
+        <v>0.03210527892224491</v>
       </c>
       <c r="G62">
-        <v>35169</v>
+        <v>36415</v>
       </c>
       <c r="H62">
-        <v>77507</v>
+        <v>78911</v>
       </c>
       <c r="I62">
-        <v>42338</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2285,28 +2285,28 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0.01873432099819183</v>
+        <v>0.02257105195894837</v>
       </c>
       <c r="C63">
-        <v>378116</v>
+        <v>241459</v>
       </c>
       <c r="D63">
-        <v>543452</v>
+        <v>402095</v>
       </c>
       <c r="E63">
-        <v>165336</v>
+        <v>160636</v>
       </c>
       <c r="F63">
-        <v>0.006950791925191879</v>
+        <v>0.02632088598329574</v>
       </c>
       <c r="G63">
-        <v>35137</v>
+        <v>36511</v>
       </c>
       <c r="H63">
-        <v>77478</v>
+        <v>78853</v>
       </c>
       <c r="I63">
-        <v>42341</v>
+        <v>42342</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2314,25 +2314,25 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.03250590711832047</v>
+        <v>0.05322739295661449</v>
       </c>
       <c r="C64">
-        <v>429752</v>
+        <v>659065</v>
       </c>
       <c r="D64">
-        <v>591258</v>
+        <v>737552</v>
       </c>
       <c r="E64">
-        <v>161506</v>
+        <v>78487</v>
       </c>
       <c r="F64">
-        <v>0.006707463413476944</v>
+        <v>0.0201522089773789</v>
       </c>
       <c r="G64">
-        <v>35041</v>
+        <v>36255</v>
       </c>
       <c r="H64">
-        <v>77537</v>
+        <v>78751</v>
       </c>
       <c r="I64">
         <v>42496</v>
@@ -2343,28 +2343,28 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0.01862265542149544</v>
+        <v>0.0568239149870351</v>
       </c>
       <c r="C65">
-        <v>350425</v>
+        <v>718738</v>
       </c>
       <c r="D65">
-        <v>510987</v>
+        <v>720389</v>
       </c>
       <c r="E65">
-        <v>160562</v>
+        <v>1651</v>
       </c>
       <c r="F65">
-        <v>0.0077177993953228</v>
+        <v>0.02216122904792428</v>
       </c>
       <c r="G65">
-        <v>35297</v>
+        <v>36063</v>
       </c>
       <c r="H65">
-        <v>77639</v>
+        <v>78559</v>
       </c>
       <c r="I65">
-        <v>42342</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2372,28 +2372,28 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0.0184604749083519</v>
+        <v>0.04422468901611865</v>
       </c>
       <c r="C66">
-        <v>346753</v>
+        <v>762355</v>
       </c>
       <c r="D66">
-        <v>520593</v>
+        <v>878220</v>
       </c>
       <c r="E66">
-        <v>173840</v>
+        <v>115865</v>
       </c>
       <c r="F66">
-        <v>0.008237075060606003</v>
+        <v>0.0278017979580909</v>
       </c>
       <c r="G66">
-        <v>35041</v>
+        <v>36639</v>
       </c>
       <c r="H66">
-        <v>77537</v>
+        <v>78975</v>
       </c>
       <c r="I66">
-        <v>42496</v>
+        <v>42336</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2401,28 +2401,28 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0.01690047979354858</v>
+        <v>0.02147486608009785</v>
       </c>
       <c r="C67">
-        <v>366187</v>
+        <v>232509</v>
       </c>
       <c r="D67">
-        <v>527615</v>
+        <v>395921</v>
       </c>
       <c r="E67">
-        <v>161428</v>
+        <v>163412</v>
       </c>
       <c r="F67">
-        <v>0.007219046354293823</v>
+        <v>0.02177799306809902</v>
       </c>
       <c r="G67">
-        <v>35297</v>
+        <v>36695</v>
       </c>
       <c r="H67">
-        <v>77793</v>
+        <v>79010</v>
       </c>
       <c r="I67">
-        <v>42496</v>
+        <v>42315</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2430,28 +2430,28 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0.024774469435215</v>
+        <v>0.05417391902301461</v>
       </c>
       <c r="C68">
-        <v>364551</v>
+        <v>429624</v>
       </c>
       <c r="D68">
-        <v>477559</v>
+        <v>589015</v>
       </c>
       <c r="E68">
-        <v>113008</v>
+        <v>159391</v>
       </c>
       <c r="F68">
-        <v>0.006293784826993942</v>
+        <v>0.02959920396097004</v>
       </c>
       <c r="G68">
-        <v>34081</v>
+        <v>36823</v>
       </c>
       <c r="H68">
-        <v>76424</v>
+        <v>79295</v>
       </c>
       <c r="I68">
-        <v>42343</v>
+        <v>42472</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2459,28 +2459,28 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0.03491738438606262</v>
+        <v>0.04709427698981017</v>
       </c>
       <c r="C69">
-        <v>362760</v>
+        <v>606981</v>
       </c>
       <c r="D69">
-        <v>599515</v>
+        <v>770603</v>
       </c>
       <c r="E69">
-        <v>236755</v>
+        <v>163622</v>
       </c>
       <c r="F69">
-        <v>0.007351085543632507</v>
+        <v>0.02124944899696857</v>
       </c>
       <c r="G69">
-        <v>34945</v>
+        <v>36639</v>
       </c>
       <c r="H69">
-        <v>77126</v>
+        <v>79135</v>
       </c>
       <c r="I69">
-        <v>42181</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2488,28 +2488,28 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.01146697252988815</v>
+        <v>0.05063139996491373</v>
       </c>
       <c r="C70">
-        <v>225770</v>
+        <v>822816</v>
       </c>
       <c r="D70">
-        <v>386650</v>
+        <v>1059984</v>
       </c>
       <c r="E70">
-        <v>160880</v>
+        <v>237168</v>
       </c>
       <c r="F70">
-        <v>0.006871465593576431</v>
+        <v>0.006971962051466107</v>
       </c>
       <c r="G70">
-        <v>34849</v>
+        <v>36127</v>
       </c>
       <c r="H70">
-        <v>77187</v>
+        <v>78469</v>
       </c>
       <c r="I70">
-        <v>42338</v>
+        <v>42342</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2517,28 +2517,28 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.01671227812767029</v>
+        <v>0.03690426598768681</v>
       </c>
       <c r="C71">
-        <v>364782</v>
+        <v>516305</v>
       </c>
       <c r="D71">
-        <v>525894</v>
+        <v>679264</v>
       </c>
       <c r="E71">
-        <v>161112</v>
+        <v>162959</v>
       </c>
       <c r="F71">
-        <v>0.006953686475753784</v>
+        <v>0.02056006307248026</v>
       </c>
       <c r="G71">
-        <v>35329</v>
+        <v>36223</v>
       </c>
       <c r="H71">
-        <v>77825</v>
+        <v>78255</v>
       </c>
       <c r="I71">
-        <v>42496</v>
+        <v>42032</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2546,25 +2546,25 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0.03243663161993027</v>
+        <v>0.04858374700415879</v>
       </c>
       <c r="C72">
-        <v>353159</v>
+        <v>422290</v>
       </c>
       <c r="D72">
-        <v>566499</v>
+        <v>583636</v>
       </c>
       <c r="E72">
-        <v>213340</v>
+        <v>161346</v>
       </c>
       <c r="F72">
-        <v>0.01221982017159462</v>
+        <v>0.01658545306418091</v>
       </c>
       <c r="G72">
-        <v>35265</v>
+        <v>35967</v>
       </c>
       <c r="H72">
-        <v>77761</v>
+        <v>78463</v>
       </c>
       <c r="I72">
         <v>42496</v>
@@ -2575,28 +2575,28 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.03365887701511383</v>
+        <v>0.04429690598044544</v>
       </c>
       <c r="C73">
-        <v>467222</v>
+        <v>579473</v>
       </c>
       <c r="D73">
-        <v>627276</v>
+        <v>741176</v>
       </c>
       <c r="E73">
-        <v>160054</v>
+        <v>161703</v>
       </c>
       <c r="F73">
-        <v>0.009038783609867096</v>
+        <v>0.02239352103788406</v>
       </c>
       <c r="G73">
-        <v>34945</v>
+        <v>35423</v>
       </c>
       <c r="H73">
-        <v>77288</v>
+        <v>77919</v>
       </c>
       <c r="I73">
-        <v>42343</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -2604,28 +2604,28 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0.02665695920586586</v>
+        <v>0.06903568306006491</v>
       </c>
       <c r="C74">
-        <v>356352</v>
+        <v>435987</v>
       </c>
       <c r="D74">
-        <v>540511</v>
+        <v>599316</v>
       </c>
       <c r="E74">
-        <v>184159</v>
+        <v>163329</v>
       </c>
       <c r="F74">
-        <v>0.01112494990229607</v>
+        <v>0.01786942407488823</v>
       </c>
       <c r="G74">
-        <v>35553</v>
+        <v>36511</v>
       </c>
       <c r="H74">
-        <v>77893</v>
+        <v>78700</v>
       </c>
       <c r="I74">
-        <v>42340</v>
+        <v>42189</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -2633,28 +2633,28 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0.05514610931277275</v>
+        <v>0.06784103100653738</v>
       </c>
       <c r="C75">
-        <v>435856</v>
+        <v>942025</v>
       </c>
       <c r="D75">
-        <v>594368</v>
+        <v>1021181</v>
       </c>
       <c r="E75">
-        <v>158512</v>
+        <v>79156</v>
       </c>
       <c r="F75">
-        <v>0.007908537983894348</v>
+        <v>0.02632019005250186</v>
       </c>
       <c r="G75">
-        <v>34841</v>
+        <v>36735</v>
       </c>
       <c r="H75">
-        <v>77004</v>
+        <v>79076</v>
       </c>
       <c r="I75">
-        <v>42163</v>
+        <v>42341</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -2662,28 +2662,28 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0.01238905265927315</v>
+        <v>0.04163539293222129</v>
       </c>
       <c r="C76">
-        <v>224305</v>
+        <v>750616</v>
       </c>
       <c r="D76">
-        <v>383125</v>
+        <v>916378</v>
       </c>
       <c r="E76">
-        <v>158820</v>
+        <v>165762</v>
       </c>
       <c r="F76">
-        <v>0.009083449840545654</v>
+        <v>0.01735922100488096</v>
       </c>
       <c r="G76">
-        <v>34649</v>
+        <v>36287</v>
       </c>
       <c r="H76">
-        <v>76963</v>
+        <v>78630</v>
       </c>
       <c r="I76">
-        <v>42314</v>
+        <v>42343</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -2691,28 +2691,28 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0.01459725573658943</v>
+        <v>0.03401235199999064</v>
       </c>
       <c r="C77">
-        <v>220055</v>
+        <v>270010</v>
       </c>
       <c r="D77">
-        <v>376945</v>
+        <v>430118</v>
       </c>
       <c r="E77">
-        <v>156890</v>
+        <v>160108</v>
       </c>
       <c r="F77">
-        <v>0.004867196083068848</v>
+        <v>0.02822655090130866</v>
       </c>
       <c r="G77">
-        <v>34817</v>
+        <v>36735</v>
       </c>
       <c r="H77">
-        <v>77156</v>
+        <v>79075</v>
       </c>
       <c r="I77">
-        <v>42339</v>
+        <v>42340</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -2720,28 +2720,28 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0.03494745120406151</v>
+        <v>0.07756722893100232</v>
       </c>
       <c r="C78">
-        <v>478023</v>
+        <v>596418</v>
       </c>
       <c r="D78">
-        <v>638457</v>
+        <v>791404</v>
       </c>
       <c r="E78">
-        <v>160434</v>
+        <v>194986</v>
       </c>
       <c r="F78">
-        <v>0.005428560078144073</v>
+        <v>0.02563956705853343</v>
       </c>
       <c r="G78">
-        <v>35009</v>
+        <v>37247</v>
       </c>
       <c r="H78">
-        <v>77353</v>
+        <v>79743</v>
       </c>
       <c r="I78">
-        <v>42344</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -2749,25 +2749,25 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0.02826141938567162</v>
+        <v>0.04967962298542261</v>
       </c>
       <c r="C79">
-        <v>354010</v>
+        <v>538916</v>
       </c>
       <c r="D79">
-        <v>512670</v>
+        <v>621383</v>
       </c>
       <c r="E79">
-        <v>158660</v>
+        <v>82467</v>
       </c>
       <c r="F79">
-        <v>0.005960129201412201</v>
+        <v>0.01952539291232824</v>
       </c>
       <c r="G79">
-        <v>34881</v>
+        <v>36319</v>
       </c>
       <c r="H79">
-        <v>77377</v>
+        <v>78815</v>
       </c>
       <c r="I79">
         <v>42496</v>
@@ -2778,28 +2778,28 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0.0291195809841156</v>
+        <v>0.03132594202179462</v>
       </c>
       <c r="C80">
-        <v>364530</v>
+        <v>415906</v>
       </c>
       <c r="D80">
-        <v>611572</v>
+        <v>652587</v>
       </c>
       <c r="E80">
-        <v>247042</v>
+        <v>236681</v>
       </c>
       <c r="F80">
-        <v>0.005190730094909668</v>
+        <v>0.02607533906120807</v>
       </c>
       <c r="G80">
-        <v>35553</v>
+        <v>36951</v>
       </c>
       <c r="H80">
-        <v>78049</v>
+        <v>79265</v>
       </c>
       <c r="I80">
-        <v>42496</v>
+        <v>42314</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -2807,28 +2807,28 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0.03039917722344398</v>
+        <v>0.07021997903939337</v>
       </c>
       <c r="C81">
-        <v>360776</v>
+        <v>641238</v>
       </c>
       <c r="D81">
-        <v>640590</v>
+        <v>803818</v>
       </c>
       <c r="E81">
-        <v>279814</v>
+        <v>162580</v>
       </c>
       <c r="F81">
-        <v>0.01174052804708481</v>
+        <v>0.02529921196401119</v>
       </c>
       <c r="G81">
-        <v>33953</v>
+        <v>35807</v>
       </c>
       <c r="H81">
-        <v>76138</v>
+        <v>78303</v>
       </c>
       <c r="I81">
-        <v>42185</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -2836,28 +2836,28 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>0.02594849094748497</v>
+        <v>0.04350384999997914</v>
       </c>
       <c r="C82">
-        <v>353774</v>
+        <v>450822</v>
       </c>
       <c r="D82">
-        <v>610249</v>
+        <v>684030</v>
       </c>
       <c r="E82">
-        <v>256475</v>
+        <v>233208</v>
       </c>
       <c r="F82">
-        <v>0.008309002965688705</v>
+        <v>0.02250672806985676</v>
       </c>
       <c r="G82">
-        <v>35073</v>
+        <v>35999</v>
       </c>
       <c r="H82">
-        <v>77569</v>
+        <v>78342</v>
       </c>
       <c r="I82">
-        <v>42496</v>
+        <v>42343</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -2865,28 +2865,28 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>0.02149039134383202</v>
+        <v>0.04871054005343467</v>
       </c>
       <c r="C83">
-        <v>351344</v>
+        <v>773485</v>
       </c>
       <c r="D83">
-        <v>506598</v>
+        <v>937858</v>
       </c>
       <c r="E83">
-        <v>155254</v>
+        <v>164373</v>
       </c>
       <c r="F83">
-        <v>0.008996099233627319</v>
+        <v>0.02073147695045918</v>
       </c>
       <c r="G83">
-        <v>34177</v>
+        <v>35903</v>
       </c>
       <c r="H83">
-        <v>76673</v>
+        <v>78243</v>
       </c>
       <c r="I83">
-        <v>42496</v>
+        <v>42340</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -2894,28 +2894,28 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>0.02430785447359085</v>
+        <v>0.07958341005723923</v>
       </c>
       <c r="C84">
-        <v>352708</v>
+        <v>1092226</v>
       </c>
       <c r="D84">
-        <v>512676</v>
+        <v>1255282</v>
       </c>
       <c r="E84">
-        <v>159968</v>
+        <v>163056</v>
       </c>
       <c r="F84">
-        <v>0.006196595728397369</v>
+        <v>0.02612848894204944</v>
       </c>
       <c r="G84">
-        <v>34145</v>
+        <v>36415</v>
       </c>
       <c r="H84">
-        <v>76641</v>
+        <v>78754</v>
       </c>
       <c r="I84">
-        <v>42496</v>
+        <v>42339</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -2923,25 +2923,25 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>0.01735591888427734</v>
+        <v>0.03312939207535237</v>
       </c>
       <c r="C85">
-        <v>362253</v>
+        <v>241310</v>
       </c>
       <c r="D85">
-        <v>523669</v>
+        <v>400195</v>
       </c>
       <c r="E85">
-        <v>161416</v>
+        <v>158885</v>
       </c>
       <c r="F85">
-        <v>0.01042203232645988</v>
+        <v>0.02958715695422143</v>
       </c>
       <c r="G85">
-        <v>35041</v>
+        <v>35551</v>
       </c>
       <c r="H85">
-        <v>77537</v>
+        <v>78047</v>
       </c>
       <c r="I85">
         <v>42496</v>
@@ -2952,25 +2952,25 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>0.02553784102201462</v>
+        <v>0.04833693208638579</v>
       </c>
       <c r="C86">
-        <v>484334</v>
+        <v>245933</v>
       </c>
       <c r="D86">
-        <v>644966</v>
+        <v>608294</v>
       </c>
       <c r="E86">
-        <v>160632</v>
+        <v>362361</v>
       </c>
       <c r="F86">
-        <v>0.009837493300437927</v>
+        <v>0.03339131898246706</v>
       </c>
       <c r="G86">
-        <v>34433</v>
+        <v>37055</v>
       </c>
       <c r="H86">
-        <v>76929</v>
+        <v>79551</v>
       </c>
       <c r="I86">
         <v>42496</v>
@@ -2981,28 +2981,28 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0.03442962467670441</v>
+        <v>0.2248019790276885</v>
       </c>
       <c r="C87">
-        <v>484931</v>
+        <v>632200</v>
       </c>
       <c r="D87">
-        <v>644239</v>
+        <v>869098</v>
       </c>
       <c r="E87">
-        <v>159308</v>
+        <v>236898</v>
       </c>
       <c r="F87">
-        <v>0.006251968443393707</v>
+        <v>0.02909202896989882</v>
       </c>
       <c r="G87">
-        <v>35225</v>
+        <v>36479</v>
       </c>
       <c r="H87">
-        <v>77542</v>
+        <v>78975</v>
       </c>
       <c r="I87">
-        <v>42317</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3010,28 +3010,28 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0.03907940536737442</v>
+        <v>0.04241986200213432</v>
       </c>
       <c r="C88">
-        <v>482332</v>
+        <v>571008</v>
       </c>
       <c r="D88">
-        <v>643964</v>
+        <v>731820</v>
       </c>
       <c r="E88">
-        <v>161632</v>
+        <v>160812</v>
       </c>
       <c r="F88">
-        <v>0.00710403174161911</v>
+        <v>0.01748521602712572</v>
       </c>
       <c r="G88">
-        <v>35169</v>
+        <v>36127</v>
       </c>
       <c r="H88">
-        <v>77665</v>
+        <v>78466</v>
       </c>
       <c r="I88">
-        <v>42496</v>
+        <v>42339</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3039,28 +3039,28 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>0.02328550815582275</v>
+        <v>0.06409234297461808</v>
       </c>
       <c r="C89">
-        <v>297966</v>
+        <v>904175</v>
       </c>
       <c r="D89">
-        <v>452865</v>
+        <v>962412</v>
       </c>
       <c r="E89">
-        <v>154899</v>
+        <v>58237</v>
       </c>
       <c r="F89">
-        <v>0.01236547157168388</v>
+        <v>0.01917144993785769</v>
       </c>
       <c r="G89">
-        <v>35745</v>
+        <v>35935</v>
       </c>
       <c r="H89">
-        <v>78241</v>
+        <v>78119</v>
       </c>
       <c r="I89">
-        <v>42496</v>
+        <v>42184</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3068,28 +3068,28 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>0.02600898221135139</v>
+        <v>0.03234614303801209</v>
       </c>
       <c r="C90">
-        <v>355683</v>
+        <v>633559</v>
       </c>
       <c r="D90">
-        <v>513099</v>
+        <v>871139</v>
       </c>
       <c r="E90">
-        <v>157416</v>
+        <v>237580</v>
       </c>
       <c r="F90">
-        <v>0.006982721388339996</v>
+        <v>0.02561562100891024</v>
       </c>
       <c r="G90">
-        <v>35297</v>
+        <v>35871</v>
       </c>
       <c r="H90">
-        <v>77636</v>
+        <v>78212</v>
       </c>
       <c r="I90">
-        <v>42339</v>
+        <v>42341</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3097,25 +3097,25 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0.05790770053863525</v>
+        <v>0.03572526597417891</v>
       </c>
       <c r="C91">
-        <v>487584</v>
+        <v>610043</v>
       </c>
       <c r="D91">
-        <v>643214</v>
+        <v>611037</v>
       </c>
       <c r="E91">
-        <v>155630</v>
+        <v>994</v>
       </c>
       <c r="F91">
-        <v>0.01051892712712288</v>
+        <v>0.02622190199326724</v>
       </c>
       <c r="G91">
-        <v>34849</v>
+        <v>36383</v>
       </c>
       <c r="H91">
-        <v>77345</v>
+        <v>78879</v>
       </c>
       <c r="I91">
         <v>42496</v>
@@ -3126,25 +3126,25 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>0.02296179905533791</v>
+        <v>0.04802544508129358</v>
       </c>
       <c r="C92">
-        <v>358714</v>
+        <v>735086</v>
       </c>
       <c r="D92">
-        <v>614645</v>
+        <v>900062</v>
       </c>
       <c r="E92">
-        <v>255931</v>
+        <v>164976</v>
       </c>
       <c r="F92">
-        <v>0.006795518100261688</v>
+        <v>0.01972697104793042</v>
       </c>
       <c r="G92">
-        <v>34913</v>
+        <v>36511</v>
       </c>
       <c r="H92">
-        <v>77409</v>
+        <v>79007</v>
       </c>
       <c r="I92">
         <v>42496</v>
@@ -3155,28 +3155,28 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.01967873051762581</v>
+        <v>0.04750331200193614</v>
       </c>
       <c r="C93">
-        <v>351938</v>
+        <v>739957</v>
       </c>
       <c r="D93">
-        <v>528466</v>
+        <v>903266</v>
       </c>
       <c r="E93">
-        <v>176528</v>
+        <v>163309</v>
       </c>
       <c r="F93">
-        <v>0.006424110382795334</v>
+        <v>0.02418878697790205</v>
       </c>
       <c r="G93">
-        <v>34945</v>
+        <v>36599</v>
       </c>
       <c r="H93">
-        <v>77441</v>
+        <v>79071</v>
       </c>
       <c r="I93">
-        <v>42496</v>
+        <v>42472</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -3184,28 +3184,28 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0.01954603940248489</v>
+        <v>0.03063388902228326</v>
       </c>
       <c r="C94">
-        <v>353535</v>
+        <v>245797</v>
       </c>
       <c r="D94">
-        <v>516671</v>
+        <v>409309</v>
       </c>
       <c r="E94">
-        <v>163136</v>
+        <v>163512</v>
       </c>
       <c r="F94">
-        <v>0.005832958966493607</v>
+        <v>0.01734669902361929</v>
       </c>
       <c r="G94">
-        <v>35137</v>
+        <v>36543</v>
       </c>
       <c r="H94">
-        <v>77477</v>
+        <v>79039</v>
       </c>
       <c r="I94">
-        <v>42340</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3213,28 +3213,28 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.03393250703811646</v>
+        <v>0.03730493504554033</v>
       </c>
       <c r="C95">
-        <v>351750</v>
+        <v>712510</v>
       </c>
       <c r="D95">
-        <v>572185</v>
+        <v>874192</v>
       </c>
       <c r="E95">
-        <v>220435</v>
+        <v>161682</v>
       </c>
       <c r="F95">
-        <v>0.007477018982172012</v>
+        <v>0.022686489042826</v>
       </c>
       <c r="G95">
-        <v>35489</v>
+        <v>36383</v>
       </c>
       <c r="H95">
-        <v>77985</v>
+        <v>78724</v>
       </c>
       <c r="I95">
-        <v>42496</v>
+        <v>42341</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3242,28 +3242,28 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0.03309835493564606</v>
+        <v>0.03081124904565513</v>
       </c>
       <c r="C96">
-        <v>485062</v>
+        <v>248636</v>
       </c>
       <c r="D96">
-        <v>641841</v>
+        <v>412396</v>
       </c>
       <c r="E96">
-        <v>156779</v>
+        <v>163760</v>
       </c>
       <c r="F96">
-        <v>0.006154399365186691</v>
+        <v>0.02829663397278637</v>
       </c>
       <c r="G96">
-        <v>34649</v>
+        <v>37279</v>
       </c>
       <c r="H96">
-        <v>77121</v>
+        <v>79775</v>
       </c>
       <c r="I96">
-        <v>42472</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3271,28 +3271,28 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0.01186535507440567</v>
+        <v>0.04351483704522252</v>
       </c>
       <c r="C97">
-        <v>228690</v>
+        <v>409038</v>
       </c>
       <c r="D97">
-        <v>391314</v>
+        <v>477253</v>
       </c>
       <c r="E97">
-        <v>162624</v>
+        <v>68215</v>
       </c>
       <c r="F97">
-        <v>0.006176035851240158</v>
+        <v>0.02772100397851318</v>
       </c>
       <c r="G97">
-        <v>34049</v>
+        <v>36031</v>
       </c>
       <c r="H97">
-        <v>76545</v>
+        <v>78219</v>
       </c>
       <c r="I97">
-        <v>42496</v>
+        <v>42188</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3300,28 +3300,28 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>0.03076743334531784</v>
+        <v>0.03876242600381374</v>
       </c>
       <c r="C98">
-        <v>471002</v>
+        <v>880411</v>
       </c>
       <c r="D98">
-        <v>631599</v>
+        <v>1017104</v>
       </c>
       <c r="E98">
-        <v>160597</v>
+        <v>136693</v>
       </c>
       <c r="F98">
-        <v>0.008289247751235962</v>
+        <v>0.01773522701114416</v>
       </c>
       <c r="G98">
-        <v>34465</v>
+        <v>36223</v>
       </c>
       <c r="H98">
-        <v>76804</v>
+        <v>78565</v>
       </c>
       <c r="I98">
-        <v>42339</v>
+        <v>42342</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3329,25 +3329,25 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>0.01816925033926964</v>
+        <v>0.0438927470240742</v>
       </c>
       <c r="C99">
-        <v>354581</v>
+        <v>770667</v>
       </c>
       <c r="D99">
-        <v>514101</v>
+        <v>932293</v>
       </c>
       <c r="E99">
-        <v>159520</v>
+        <v>161626</v>
       </c>
       <c r="F99">
-        <v>0.004804685711860657</v>
+        <v>0.02566265396308154</v>
       </c>
       <c r="G99">
-        <v>34849</v>
+        <v>36447</v>
       </c>
       <c r="H99">
-        <v>77345</v>
+        <v>78943</v>
       </c>
       <c r="I99">
         <v>42496</v>
@@ -3358,25 +3358,25 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>0.03004952520132065</v>
+        <v>0.01920294598676264</v>
       </c>
       <c r="C100">
-        <v>496858</v>
+        <v>226019</v>
       </c>
       <c r="D100">
-        <v>660554</v>
+        <v>386229</v>
       </c>
       <c r="E100">
-        <v>163696</v>
+        <v>160210</v>
       </c>
       <c r="F100">
-        <v>0.006433773785829544</v>
+        <v>0.02698576299007982</v>
       </c>
       <c r="G100">
-        <v>34977</v>
+        <v>35871</v>
       </c>
       <c r="H100">
-        <v>77473</v>
+        <v>78367</v>
       </c>
       <c r="I100">
         <v>42496</v>
@@ -3387,25 +3387,25 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>0.03429126366972923</v>
+        <v>0.03565889701712877</v>
       </c>
       <c r="C101">
-        <v>413868</v>
+        <v>677328</v>
       </c>
       <c r="D101">
-        <v>573900</v>
+        <v>838103</v>
       </c>
       <c r="E101">
-        <v>160032</v>
+        <v>160775</v>
       </c>
       <c r="F101">
-        <v>0.006314888596534729</v>
+        <v>0.01726676500402391</v>
       </c>
       <c r="G101">
-        <v>34209</v>
+        <v>35231</v>
       </c>
       <c r="H101">
-        <v>76705</v>
+        <v>77727</v>
       </c>
       <c r="I101">
         <v>42496</v>

</xml_diff>